<commit_message>
Commint experiments on datatset-3
</commit_message>
<xml_diff>
--- a/ExperimentReport/DataSet-3/Experiment Report.xlsx
+++ b/ExperimentReport/DataSet-3/Experiment Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\source\repos\neocortexapi-classification\ExperimentReport\DataSet-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFE7076-589F-496F-BFD5-81D3A2B76686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8569A337-1196-497B-86A1-D32F9D202472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Experiment Number</t>
   </si>
@@ -57,9 +57,6 @@
     <t>HTM Parameters</t>
   </si>
   <si>
-    <t>Result Information</t>
-  </si>
-  <si>
     <t>Experiment Github URL</t>
   </si>
   <si>
@@ -69,37 +66,34 @@
     <t>32x32</t>
   </si>
   <si>
-    <t>The Micro and Macro corelation are low</t>
-  </si>
-  <si>
-    <t>The Micro and Macro corelation are high, but the micro corelation's min value is less than the macro corelation max value</t>
-  </si>
-  <si>
-    <t>cells per coloumn</t>
-  </si>
-  <si>
-    <t>https://github.com/GurunagSai/neocortexapi-classification/tree/GurunagSai/ExperimentReport/DataSet-3/output-02.png</t>
-  </si>
-  <si>
-    <t>https://github.com/GurunagSai/neocortexapi-classification/tree/GurunagSai/ExperimentReport/DataSet-3/output-01.png</t>
-  </si>
-  <si>
-    <t>https://github.com/GurunagSai/neocortexapi-classification/tree/GurunagSai/ExperimentReport/DataSet-3/output-03.png</t>
-  </si>
-  <si>
-    <t>https://github.com/GurunagSai/neocortexapi-classification/tree/GurunagSai/ExperimentReport/DataSet-3/output-04.png</t>
-  </si>
-  <si>
-    <t>https://github.com/GurunagSai/neocortexapi-classification/tree/GurunagSai/ExperimentReport/DataSet-3/output-05.png</t>
-  </si>
-  <si>
-    <t>https://github.com/GurunagSai/neocortexapi-classification/tree/GurunagSai/ExperimentReport/DataSet-3/output-06.png</t>
-  </si>
-  <si>
-    <t>https://github.com/GurunagSai/neocortexapi-classification/tree/GurunagSai/ExperimentReport/DataSet-3/output-07.png</t>
-  </si>
-  <si>
-    <t>https://github.com/GurunagSai/neocortexapi-classification/tree/GurunagSai/ExperimentReport/DataSet-3/output-08.png</t>
+    <t>https://github.com/GurunagSai/neocortexapi-classification/blob/GurunagSai/ExperimentReport/DataSet-3/output-01.png</t>
+  </si>
+  <si>
+    <t>https://github.com/GurunagSai/neocortexapi-classification/blob/GurunagSai/ExperimentReport/DataSet-3/output-02.png</t>
+  </si>
+  <si>
+    <t>https://github.com/GurunagSai/neocortexapi-classification/blob/GurunagSai/ExperimentReport/DataSet-3/output-03.png</t>
+  </si>
+  <si>
+    <t>https://github.com/GurunagSai/neocortexapi-classification/blob/GurunagSai/ExperimentReport/DataSet-3/output-04.png</t>
+  </si>
+  <si>
+    <t>https://github.com/GurunagSai/neocortexapi-classification/blob/GurunagSai/ExperimentReport/DataSet-3/output-05.png</t>
+  </si>
+  <si>
+    <t>https://github.com/GurunagSai/neocortexapi-classification/blob/GurunagSai/ExperimentReport/DataSet-3/output-06.png</t>
+  </si>
+  <si>
+    <t>Result(micro and macro corelation)</t>
+  </si>
+  <si>
+    <t>micro corelation min is greater than macro corelation max, but the values are around 50%</t>
+  </si>
+  <si>
+    <t>micro corr and macro corr condition did not meet</t>
+  </si>
+  <si>
+    <t>micro corelation min is greater than macro corelation max, but the values are around 40%</t>
   </si>
 </sst>
 </file>
@@ -191,7 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -217,7 +211,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -499,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,14 +507,14 @@
     <col min="5" max="5" width="12.5703125" style="2" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="28.28515625" style="2" customWidth="1"/>
-    <col min="8" max="9" width="18.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="70.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="59" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="8" max="8" width="18.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="70.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="71.7109375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -535,15 +528,14 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="J1" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="K1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -567,15 +559,12 @@
         <v>7</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="J2" s="10"/>
       <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-    </row>
-    <row r="3" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -598,22 +587,19 @@
         <v>-1</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="2">
-        <v>16</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -636,24 +622,21 @@
         <v>-1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="2">
-        <v>16</v>
-      </c>
-      <c r="J4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -662,7 +645,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2">
         <v>0.5</v>
@@ -674,24 +657,21 @@
         <v>-1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="2">
-        <v>16</v>
-      </c>
-      <c r="J5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -700,7 +680,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="2">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2">
         <v>0.5</v>
@@ -712,24 +692,21 @@
         <v>-1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="11">
+        <v>12</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -738,36 +715,30 @@
         <v>0</v>
       </c>
       <c r="D7" s="2">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E7" s="2">
         <v>0.5</v>
       </c>
       <c r="F7" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G7" s="2">
         <v>-1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="11">
-        <v>16</v>
-      </c>
-      <c r="J7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
@@ -776,157 +747,78 @@
         <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2">
         <v>0.5</v>
       </c>
       <c r="F8" s="2">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="G8" s="2">
         <v>-1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="11">
-        <v>16</v>
-      </c>
-      <c r="J8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>16</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="G9" s="2">
-        <v>-1</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="11">
-        <v>16</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>16</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G10" s="2">
-        <v>-1</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="11">
-        <v>16</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K20" s="3"/>
+      <c r="I8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J20" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B1:I1"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="J1:J2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" xr:uid="{F2E518D1-5C54-4BD8-A217-0A9F30B9AF15}"/>
-    <hyperlink ref="K8" r:id="rId2" xr:uid="{55FE29AC-AFA0-4119-A22A-62EDF1E3D072}"/>
-    <hyperlink ref="K9" r:id="rId3" xr:uid="{C103260B-DF1B-4A14-A1DB-DCB3B47D4D14}"/>
-    <hyperlink ref="K10" r:id="rId4" xr:uid="{529C8DBD-6618-40C1-A828-DE6A61CA8E1E}"/>
-    <hyperlink ref="K7" r:id="rId5" xr:uid="{3FD2A608-E84F-438E-98D0-7CFA896EDD32}"/>
-    <hyperlink ref="K6" r:id="rId6" xr:uid="{8039A4B1-C904-4CD8-8B79-D41885D047EE}"/>
-    <hyperlink ref="K5" r:id="rId7" xr:uid="{EB8D6065-9024-4590-A4AD-E0836393B8C4}"/>
-    <hyperlink ref="K4" r:id="rId8" xr:uid="{C49A80D8-8B80-415F-A76D-42FFA54F24EB}"/>
+    <hyperlink ref="J4" r:id="rId1" xr:uid="{23E8D282-0CF1-47BE-9184-87E57E04576B}"/>
+    <hyperlink ref="J5" r:id="rId2" xr:uid="{7086C9C0-57BA-4BE3-8654-F1C81ED05F15}"/>
+    <hyperlink ref="J6" r:id="rId3" xr:uid="{4C0EA918-217D-454C-BAD8-CA5823FA9DD6}"/>
+    <hyperlink ref="J7" r:id="rId4" xr:uid="{0ED0C533-E2F3-4C3F-9F85-83EB382322A2}"/>
+    <hyperlink ref="J8" r:id="rId5" xr:uid="{BABAE635-3546-41A2-A1B2-8A00556CF939}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding experiments on potential radius and local area density
</commit_message>
<xml_diff>
--- a/ExperimentReport/DataSet-3/Experiment Report.xlsx
+++ b/ExperimentReport/DataSet-3/Experiment Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\source\repos\neocortexapi-classification\ExperimentReport\DataSet-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8569A337-1196-497B-86A1-D32F9D202472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CB3502-F29B-49F1-B115-8C73AF5CD684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Experiment Number</t>
   </si>
@@ -94,6 +94,21 @@
   </si>
   <si>
     <t>micro corelation min is greater than macro corelation max, but the values are around 40%</t>
+  </si>
+  <si>
+    <t>micro corelation min is greater than macro corelation max</t>
+  </si>
+  <si>
+    <t>micro corelation min is greater than macro corelation max (Current best output)</t>
+  </si>
+  <si>
+    <t>https://github.com/GurunagSai/neocortexapi-classification/blob/GurunagSai/ExperimentReport/DataSet-3/output-07.png</t>
+  </si>
+  <si>
+    <t>https://github.com/GurunagSai/neocortexapi-classification/blob/GurunagSai/ExperimentReport/DataSet-3/output-08.png</t>
+  </si>
+  <si>
+    <t>https://github.com/GurunagSai/neocortexapi-classification/blob/GurunagSai/ExperimentReport/DataSet-3/output-09.png</t>
   </si>
 </sst>
 </file>
@@ -494,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +651,7 @@
     </row>
     <row r="5" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -671,7 +686,7 @@
     </row>
     <row r="6" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -706,7 +721,7 @@
     </row>
     <row r="7" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -735,10 +750,13 @@
       <c r="J7" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="K7" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
@@ -767,18 +785,149 @@
       <c r="J8" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="K8" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J9" s="3"/>
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J10" s="3"/>
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J11" s="3"/>
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="G11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J12" s="3"/>
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="G12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J13" s="3"/>
@@ -817,8 +966,12 @@
     <hyperlink ref="J6" r:id="rId3" xr:uid="{4C0EA918-217D-454C-BAD8-CA5823FA9DD6}"/>
     <hyperlink ref="J7" r:id="rId4" xr:uid="{0ED0C533-E2F3-4C3F-9F85-83EB382322A2}"/>
     <hyperlink ref="J8" r:id="rId5" xr:uid="{BABAE635-3546-41A2-A1B2-8A00556CF939}"/>
+    <hyperlink ref="J9" r:id="rId6" xr:uid="{5D278D32-22F3-4CC5-9F67-0793F36D72D4}"/>
+    <hyperlink ref="J10" r:id="rId7" xr:uid="{DCC1C29F-5E12-4663-B6BF-FDB9A6C03036}"/>
+    <hyperlink ref="J11" r:id="rId8" xr:uid="{A52644CA-DDDD-4EB5-8CDD-2950E83A8BBA}"/>
+    <hyperlink ref="J12" r:id="rId9" xr:uid="{B3EC1396-D5E1-4E13-A449-F96517A8627C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding experiments on NumActiveColPerInhArea and GlobalInhibition parameters
</commit_message>
<xml_diff>
--- a/ExperimentReport/DataSet-3/Experiment Report.xlsx
+++ b/ExperimentReport/DataSet-3/Experiment Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\source\repos\neocortexapi-classification\ExperimentReport\DataSet-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFCCF38-8B8F-4F75-908F-341071EFDEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BE9D06-2312-4EED-AB26-7F45F014B1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7305" yWindow="2565" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="2565" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="75">
   <si>
     <t>Experiment Number</t>
   </si>
@@ -92,18 +92,6 @@
 macro corelation(91-34%) micro corelation(93-67%)</t>
   </si>
   <si>
-    <t>circle-rectangle macro correlation is high
-macro corelation(88-18.8%) micro corelation(96-79%)</t>
-  </si>
-  <si>
-    <t>Valid output
-macro corelation(54-0%) micro corelation(94-63%)</t>
-  </si>
-  <si>
-    <t>, 
-macro corelation(36-1.8%) micro corelation(81-40%)</t>
-  </si>
-  <si>
     <t>circle-rectangle macro correlation is high, 
 macro corelation(80-43%) micro corelation(94-74%)</t>
   </si>
@@ -113,24 +101,193 @@
   </si>
   <si>
     <t>Both macro and micro corelation are high</t>
+  </si>
+  <si>
+    <t>output-07</t>
+  </si>
+  <si>
+    <t>output-08</t>
+  </si>
+  <si>
+    <t>output-09</t>
+  </si>
+  <si>
+    <t>output-10</t>
+  </si>
+  <si>
+    <t>output-12</t>
+  </si>
+  <si>
+    <t>circle-rectangle macro correlation is high
+macro corelation(95-56%) micro corelation(96.7-88%)</t>
+  </si>
+  <si>
+    <t>valid output but macro corelation are higher
+macro corelation(82-64%) micro corelation(99-92%)</t>
+  </si>
+  <si>
+    <t>valid output but macro corelation are higher
+macro corelation(89-72%) micro corelation(99-93%)</t>
+  </si>
+  <si>
+    <t>valid output but macro corelation are higher
+macro corelation(97-90%) micro corelation(100-97%)</t>
+  </si>
+  <si>
+    <t>valid, circle-rectangle macro correlation is high
+macro corelation(88-18.8%) micro corelation(96-79%)</t>
+  </si>
+  <si>
+    <t>valid, circle-rectangle macro correlation is high
+macro corelation(80-40%) micro corelation(96-85%)</t>
+  </si>
+  <si>
+    <t>output-13</t>
+  </si>
+  <si>
+    <t>output-14</t>
+  </si>
+  <si>
+    <t>output-15</t>
+  </si>
+  <si>
+    <t>output-17</t>
+  </si>
+  <si>
+    <t>output-18</t>
+  </si>
+  <si>
+    <t>output-19</t>
+  </si>
+  <si>
+    <t>output-20</t>
+  </si>
+  <si>
+    <t>circle-rectangle macro correlation is high
+macro corelation(91-69%) micro corelation(97-93%)</t>
+  </si>
+  <si>
+    <t>circle-rectangle macro correlation is high
+macro corelation(89-76%) micro corelation(99-91%)</t>
+  </si>
+  <si>
+    <t>circle-rectangle macro correlation is high,
+macro corelation(36-1.8%) micro corelation(81-40%)</t>
+  </si>
+  <si>
+    <t>Valid output (best so far)
+macro corelation(54-0%) micro corelation(94-63%)</t>
+  </si>
+  <si>
+    <t>Valid output
+macro corelation(57-17%) micro corelation(89-64%)</t>
+  </si>
+  <si>
+    <t>output-21</t>
+  </si>
+  <si>
+    <t>output-22</t>
+  </si>
+  <si>
+    <t>output-23</t>
+  </si>
+  <si>
+    <t>output-24</t>
+  </si>
+  <si>
+    <t>output-25</t>
+  </si>
+  <si>
+    <t>32x32 
+(active col:10)</t>
+  </si>
+  <si>
+    <t>32x32 
+(active col:20)</t>
+  </si>
+  <si>
+    <t>32x32 
+(active col:50)</t>
+  </si>
+  <si>
+    <t>output-26</t>
+  </si>
+  <si>
+    <t>output-27</t>
+  </si>
+  <si>
+    <t>32x32 
+(active col:100)</t>
+  </si>
+  <si>
+    <t>output-28</t>
+  </si>
+  <si>
+    <t>output-29</t>
+  </si>
+  <si>
+    <t>output-31</t>
+  </si>
+  <si>
+    <t>output-32</t>
+  </si>
+  <si>
+    <t>32x32 
+(active col:avg 55)</t>
+  </si>
+  <si>
+    <t>32x32 
+(active col: 106)</t>
+  </si>
+  <si>
+    <t>32x32 
+(active col: 100)</t>
+  </si>
+  <si>
+    <t>output-30</t>
+  </si>
+  <si>
+    <t>64x64
+(active col: avg 406)</t>
+  </si>
+  <si>
+    <t>output-33</t>
+  </si>
+  <si>
+    <t>Both macro and micro corelation are low and almost equal</t>
+  </si>
+  <si>
+    <t>Valid output
+macro corelation(57-0%) micro corelation(100-68%)</t>
+  </si>
+  <si>
+    <t>Both macro and micro corelation are almost equal</t>
+  </si>
+  <si>
+    <t>corelation values are low and almost equal
+macro corelation(32-1%) micro corelation(68-27%)</t>
+  </si>
+  <si>
+    <t>circle-rectangle macro correlation is high
+macro corelation(44-4%) micro corelation(82-42%)</t>
+  </si>
+  <si>
+    <t>circle-rectangle macro correlation is high
+macro corelation(90-41%) micro corelation(97-80%)</t>
+  </si>
+  <si>
+    <t>circle-rectangle macro correlation is high
+macro corelation(45-3%) micro corelation(82-41%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,21 +357,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -230,9 +384,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -511,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="G25" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,14 +678,14 @@
     <col min="3" max="3" width="15.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="28.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="70.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
     <col min="9" max="9" width="71.7109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -541,34 +695,34 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="11"/>
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -593,7 +747,7 @@
       <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -622,11 +776,11 @@
       <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -651,11 +805,11 @@
       <c r="G5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -680,11 +834,11 @@
       <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" t="s">
         <v>14</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -709,11 +863,11 @@
       <c r="G7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" t="s">
         <v>15</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -738,7 +892,7 @@
       <c r="G8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" t="s">
         <v>16</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -767,7 +921,12 @@
       <c r="G9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="3"/>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -791,7 +950,12 @@
       <c r="G10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="3"/>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -815,7 +979,12 @@
       <c r="G11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="3"/>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -839,7 +1008,12 @@
       <c r="G12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -863,11 +1037,11 @@
       <c r="G13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" t="s">
         <v>17</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -892,7 +1066,12 @@
       <c r="G14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="3"/>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -916,7 +1095,12 @@
       <c r="G15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="3"/>
+      <c r="H15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -940,7 +1124,12 @@
       <c r="G16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="3"/>
+      <c r="H16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -964,7 +1153,12 @@
       <c r="G17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="3"/>
+      <c r="H17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -988,11 +1182,11 @@
       <c r="G18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" t="s">
         <v>18</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1017,7 +1211,12 @@
       <c r="G19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="3"/>
+      <c r="H19" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -1041,7 +1240,12 @@
       <c r="G20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="3"/>
+      <c r="H20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -1065,7 +1269,12 @@
       <c r="G21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="3"/>
+      <c r="H21" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -1089,7 +1298,389 @@
       <c r="G22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="3"/>
+      <c r="H22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="E23" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" t="s">
+        <v>47</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <v>30</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E24" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <v>30</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>30</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E26" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <v>30</v>
+      </c>
+      <c r="D27" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E27" s="2">
+        <v>10</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>30</v>
+      </c>
+      <c r="D28" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E28" s="2">
+        <v>20</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>30</v>
+      </c>
+      <c r="D29" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E29" s="2">
+        <v>50</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <v>30</v>
+      </c>
+      <c r="D30" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E30" s="2">
+        <v>100</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2">
+        <v>30</v>
+      </c>
+      <c r="D31" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E31" s="2">
+        <v>10</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32" s="2">
+        <v>30</v>
+      </c>
+      <c r="D32" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E32" s="2">
+        <v>50</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C33" s="2">
+        <v>30</v>
+      </c>
+      <c r="D33" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E33" s="2">
+        <v>100</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2">
+        <v>20</v>
+      </c>
+      <c r="D34" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E34" s="2">
+        <v>100</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2">
+        <v>30</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E35" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Updating code for image prediction
</commit_message>
<xml_diff>
--- a/ExperimentReport/DataSet-3/Experiment Report.xlsx
+++ b/ExperimentReport/DataSet-3/Experiment Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\source\repos\neocortexapi-classification\ExperimentReport\DataSet-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BE9D06-2312-4EED-AB26-7F45F014B1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42508FC0-5C74-4D11-9D02-AF76D47A5226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2565" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="77">
   <si>
     <t>Experiment Number</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>32x32</t>
-  </si>
-  <si>
-    <t>Result(micro and macro corelation)</t>
   </si>
   <si>
     <t>output-01</t>
@@ -175,10 +172,6 @@
 macro corelation(36-1.8%) micro corelation(81-40%)</t>
   </si>
   <si>
-    <t>Valid output (best so far)
-macro corelation(54-0%) micro corelation(94-63%)</t>
-  </si>
-  <si>
     <t>Valid output
 macro corelation(57-17%) micro corelation(89-64%)</t>
   </si>
@@ -278,6 +271,20 @@
   <si>
     <t>circle-rectangle macro correlation is high
 macro corelation(45-3%) micro corelation(82-41%)</t>
+  </si>
+  <si>
+    <t>Valid output 
+macro corelation(54-0%) micro corelation(94-63%)</t>
+  </si>
+  <si>
+    <t>output-34</t>
+  </si>
+  <si>
+    <t>valid output, circle-rectangle macro correlation is high
+macro corelation(57-5%) micro corelation(94-61%)</t>
+  </si>
+  <si>
+    <t>Result(micro and macro corelation where the percentages refer to the maximun and minimum values from all the shapes)</t>
   </si>
 </sst>
 </file>
@@ -665,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G25" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,7 +706,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -748,10 +755,10 @@
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -777,10 +784,10 @@
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -806,10 +813,10 @@
         <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -835,10 +842,10 @@
         <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -864,10 +871,10 @@
         <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -893,10 +900,10 @@
         <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -922,10 +929,10 @@
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -951,10 +958,10 @@
         <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -980,10 +987,10 @@
         <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1009,10 +1016,10 @@
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1038,10 +1045,10 @@
         <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1067,10 +1074,10 @@
         <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1096,10 +1103,10 @@
         <v>8</v>
       </c>
       <c r="H15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1125,10 +1132,10 @@
         <v>8</v>
       </c>
       <c r="H16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1154,10 +1161,10 @@
         <v>8</v>
       </c>
       <c r="H17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1183,10 +1190,10 @@
         <v>8</v>
       </c>
       <c r="H18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1212,10 +1219,10 @@
         <v>8</v>
       </c>
       <c r="H19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1241,10 +1248,10 @@
         <v>8</v>
       </c>
       <c r="H20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1270,10 +1277,10 @@
         <v>8</v>
       </c>
       <c r="H21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1299,10 +1306,10 @@
         <v>8</v>
       </c>
       <c r="H22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1328,10 +1335,10 @@
         <v>8</v>
       </c>
       <c r="H23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1357,10 +1364,10 @@
         <v>8</v>
       </c>
       <c r="H24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1386,10 +1393,10 @@
         <v>8</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1415,10 +1422,10 @@
         <v>8</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1438,16 +1445,16 @@
         <v>10</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1467,16 +1474,16 @@
         <v>20</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="I28" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1496,16 +1503,16 @@
         <v>50</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="I29" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1525,16 +1532,16 @@
         <v>100</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1554,16 +1561,16 @@
         <v>10</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1583,16 +1590,16 @@
         <v>50</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1612,16 +1619,16 @@
         <v>100</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1641,16 +1648,16 @@
         <v>100</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1670,16 +1677,45 @@
         <v>-1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I35" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36" s="2">
+        <v>30</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E36" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="5" t="s">
         <v>74</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding comments for the prediction code
</commit_message>
<xml_diff>
--- a/ExperimentReport/DataSet-3/Experiment Report.xlsx
+++ b/ExperimentReport/DataSet-3/Experiment Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\source\repos\neocortexapi-classification\ExperimentReport\DataSet-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42508FC0-5C74-4D11-9D02-AF76D47A5226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D41F6C-AE66-44FA-8E38-7F378BC8D028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="2565" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="79">
   <si>
     <t>Experiment Number</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>InputDimensions</t>
-  </si>
-  <si>
-    <t>Experiment Github URL</t>
   </si>
   <si>
     <t>64x64</t>
@@ -123,22 +120,6 @@
 macro corelation(82-64%) micro corelation(99-92%)</t>
   </si>
   <si>
-    <t>valid output but macro corelation are higher
-macro corelation(89-72%) micro corelation(99-93%)</t>
-  </si>
-  <si>
-    <t>valid output but macro corelation are higher
-macro corelation(97-90%) micro corelation(100-97%)</t>
-  </si>
-  <si>
-    <t>valid, circle-rectangle macro correlation is high
-macro corelation(88-18.8%) micro corelation(96-79%)</t>
-  </si>
-  <si>
-    <t>valid, circle-rectangle macro correlation is high
-macro corelation(80-40%) micro corelation(96-85%)</t>
-  </si>
-  <si>
     <t>output-13</t>
   </si>
   <si>
@@ -285,14 +266,68 @@
   </si>
   <si>
     <t>Result(micro and macro corelation where the percentages refer to the maximun and minimum values from all the shapes)</t>
+  </si>
+  <si>
+    <t>Experiment output image(Github URL- https://github.com/GurunagSai/neocortexapi-classification/tree/pre-main/MyProject/Dataset%20Reports/Dataset-GurunagSai)</t>
+  </si>
+  <si>
+    <t>output-35</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BEST OUTPUT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,
+macro corelation(46-4%) micro corelation(87-47%)</t>
+    </r>
+  </si>
+  <si>
+    <t>circle-rectangle macro correlation is high
+macro corelation(80-40%) micro corelation(96-85%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> circle-rectangle macro correlation is high
+macro corelation(88-18.8%) micro corelation(96-79%)</t>
+  </si>
+  <si>
+    <t>macro corelation are higher
+macro corelation(97-90%) micro corelation(100-97%)</t>
+  </si>
+  <si>
+    <t>macro corelation are higher
+macro corelation(89-72%) micro corelation(99-93%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -391,7 +426,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +724,7 @@
     <col min="5" max="5" width="28.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="65.28515625" customWidth="1"/>
     <col min="9" max="9" width="71.7109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -703,13 +740,13 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="11" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="4" t="s">
         <v>4</v>
@@ -749,16 +786,16 @@
         <v>-1</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -778,16 +815,16 @@
         <v>-1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -807,16 +844,16 @@
         <v>-1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -836,16 +873,16 @@
         <v>-1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -865,16 +902,16 @@
         <v>-1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -894,16 +931,16 @@
         <v>-1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -923,16 +960,16 @@
         <v>-1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -952,16 +989,16 @@
         <v>-1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -981,16 +1018,16 @@
         <v>-1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1010,16 +1047,16 @@
         <v>-1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1039,16 +1076,16 @@
         <v>-1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1068,16 +1105,16 @@
         <v>-1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1097,16 +1134,16 @@
         <v>-1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1126,16 +1163,16 @@
         <v>-1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H16" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1155,16 +1192,16 @@
         <v>-1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H17" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1184,16 +1221,16 @@
         <v>-1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1213,16 +1250,16 @@
         <v>-1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H19" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1242,16 +1279,16 @@
         <v>-1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H20" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1271,16 +1308,16 @@
         <v>-1</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H21" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1300,16 +1337,16 @@
         <v>-1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H22" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1329,16 +1366,16 @@
         <v>-1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H23" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1358,16 +1395,16 @@
         <v>-1</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H24" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1387,16 +1424,16 @@
         <v>-1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1416,16 +1453,16 @@
         <v>-1</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1445,16 +1482,16 @@
         <v>10</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1474,16 +1511,16 @@
         <v>20</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1503,16 +1540,16 @@
         <v>50</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1532,16 +1569,16 @@
         <v>100</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1561,16 +1598,16 @@
         <v>10</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1590,16 +1627,16 @@
         <v>50</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1619,16 +1656,16 @@
         <v>100</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1648,16 +1685,16 @@
         <v>100</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1677,16 +1714,16 @@
         <v>-1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1706,16 +1743,45 @@
         <v>-1</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H36" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
+        <v>30</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="E37" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding experiments on potential radius=10
</commit_message>
<xml_diff>
--- a/ExperimentReport/DataSet-3/Experiment Report.xlsx
+++ b/ExperimentReport/DataSet-3/Experiment Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\source\repos\neocortexapi-classification\ExperimentReport\DataSet-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D41F6C-AE66-44FA-8E38-7F378BC8D028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041C7DA6-3812-4AE6-8D48-BF20AE2E42EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2565" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3855" yWindow="4440" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="188">
   <si>
     <t>Experiment Number</t>
   </si>
@@ -40,12 +40,6 @@
   </si>
   <si>
     <t>Global Inhibition</t>
-  </si>
-  <si>
-    <t>ColumnDimensions</t>
-  </si>
-  <si>
-    <t>InputDimensions</t>
   </si>
   <si>
     <t>64x64</t>
@@ -266,9 +260,6 @@
   </si>
   <si>
     <t>Result(micro and macro corelation where the percentages refer to the maximun and minimum values from all the shapes)</t>
-  </si>
-  <si>
-    <t>Experiment output image(Github URL- https://github.com/GurunagSai/neocortexapi-classification/tree/pre-main/MyProject/Dataset%20Reports/Dataset-GurunagSai)</t>
   </si>
   <si>
     <t>output-35</t>
@@ -312,6 +303,416 @@
   <si>
     <t>macro corelation are higher
 macro corelation(89-72%) micro corelation(99-93%)</t>
+  </si>
+  <si>
+    <t>Experiment output (Github URL-https://github.com/GurunagSai/neocortexapi-classification/tree/main/MyProject/Dataset%20Reports/Dataset-GurunagSai/OutputFolder)</t>
+  </si>
+  <si>
+    <t>output-36</t>
+  </si>
+  <si>
+    <t>output-37</t>
+  </si>
+  <si>
+    <t>output-38</t>
+  </si>
+  <si>
+    <t>output-39</t>
+  </si>
+  <si>
+    <t>output-40</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 110</t>
+  </si>
+  <si>
+    <t>proper output but
+variance between max and min for both micro and macro corelation are high</t>
+  </si>
+  <si>
+    <t>proper output but the variance is high
+the micro correlation is 85-65% and macro is 64-34%</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 300</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 700</t>
+  </si>
+  <si>
+    <t>output-41</t>
+  </si>
+  <si>
+    <t>output-42</t>
+  </si>
+  <si>
+    <t>output-43</t>
+  </si>
+  <si>
+    <t>output-44</t>
+  </si>
+  <si>
+    <t>output-45</t>
+  </si>
+  <si>
+    <t>output-46</t>
+  </si>
+  <si>
+    <t>output-47</t>
+  </si>
+  <si>
+    <t>output-48</t>
+  </si>
+  <si>
+    <t>output-49</t>
+  </si>
+  <si>
+    <t>output-50</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 900</t>
+  </si>
+  <si>
+    <t>Both the micro and macro correlation are high but variance is less(90's-75's% for both)</t>
+  </si>
+  <si>
+    <t>Both macro(96-94) and micro(100-96) corelation are higher</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 990</t>
+  </si>
+  <si>
+    <t>Both macro(99-99) and micro(100-99) corelation are higher</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 100</t>
+  </si>
+  <si>
+    <t>circle - rectangle macro is high(85)
+micro(95-70) and macro (85-26)</t>
+  </si>
+  <si>
+    <t>circle - rectangle macro is high(87)
+micro(98-89) and macro (87-51)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 512</t>
+  </si>
+  <si>
+    <t>macro corelation is higher for cirlce-rectangle
+micro (96-83) and macro (86-65)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 716</t>
+  </si>
+  <si>
+    <t>Both macro(94-85) and micro(100-94) corelation are higher</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 921</t>
+  </si>
+  <si>
+    <t>Both macro(100-98) and micro(100-97) corelation are higher</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 134</t>
+  </si>
+  <si>
+    <t>The variance in micro corelation is more
+micro(85-40) and macro(52-17)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 422</t>
+  </si>
+  <si>
+    <t>30
+inh radius: 4</t>
+  </si>
+  <si>
+    <t>valid output
+micro(92-75) and macro(68-45)</t>
+  </si>
+  <si>
+    <t>output-51</t>
+  </si>
+  <si>
+    <t>output-52</t>
+  </si>
+  <si>
+    <t>output-53</t>
+  </si>
+  <si>
+    <t>output-54</t>
+  </si>
+  <si>
+    <t>output-55</t>
+  </si>
+  <si>
+    <t>circle0__circle1
+input sim:82.71%</t>
+  </si>
+  <si>
+    <t>rectangle0_rectangle_1
+input sim: 90.9%</t>
+  </si>
+  <si>
+    <t>triangle0__triangle1
+input sim: 81.87%</t>
+  </si>
+  <si>
+    <t>image1 vs image2 sdr corelations in %</t>
+  </si>
+  <si>
+    <t>InputDimensions
+(pixel x pixel)</t>
+  </si>
+  <si>
+    <t>ColumnDimensions
+(2D topology)</t>
+  </si>
+  <si>
+    <t>50
+inh radius: 4</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 750</t>
+  </si>
+  <si>
+    <t>macro correlation is high
+macro(88-79) and micro(96-86)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80
+inh radius: 4 </t>
+  </si>
+  <si>
+    <t>macro correlation is high
+macro(87-78) and micro(96-86)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100
+inh radius:4 </t>
+  </si>
+  <si>
+    <t>10
+inh radius:4</t>
+  </si>
+  <si>
+    <t>20
+inh radius: 4</t>
+  </si>
+  <si>
+    <t>40
+inh radius: 4</t>
+  </si>
+  <si>
+    <t>output-56</t>
+  </si>
+  <si>
+    <t>output-57</t>
+  </si>
+  <si>
+    <t>output-58</t>
+  </si>
+  <si>
+    <t>output-59</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 250</t>
+  </si>
+  <si>
+    <t>The variance in micro corelation is more
+micro(87-61) and macro(64-29)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 720</t>
+  </si>
+  <si>
+    <t>macro correlation is high
+micro(95-84) and macro(87-72)</t>
+  </si>
+  <si>
+    <t>35
+inh radius: 4</t>
+  </si>
+  <si>
+    <t>output-60</t>
+  </si>
+  <si>
+    <t>10
+inh radius: 32</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 10</t>
+  </si>
+  <si>
+    <t>variance is very high
+micro(90-10) and macro (10-0)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 600</t>
+  </si>
+  <si>
+    <t>macro is high
+micro(94-79) and macro(78-53)</t>
+  </si>
+  <si>
+    <t>20
+inh radius: 32</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 20</t>
+  </si>
+  <si>
+    <t>variance is very high
+micro(95-35) and macro (40-0)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 30</t>
+  </si>
+  <si>
+    <t>30
+inh radius: 32</t>
+  </si>
+  <si>
+    <t>variance is very high
+micro(96-53) and macro (54-0)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 40</t>
+  </si>
+  <si>
+    <t>40
+inh radius: 32</t>
+  </si>
+  <si>
+    <t>variance is very high
+micro(95-60) and macro (67.5-0)</t>
+  </si>
+  <si>
+    <t>50
+inh radius: 32</t>
+  </si>
+  <si>
+    <t>80
+inh radius: 32</t>
+  </si>
+  <si>
+    <t>100
+inh radius: 32</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 50</t>
+  </si>
+  <si>
+    <t>variance is very high
+micro(90-60) and macro (72-0)</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 80</t>
+  </si>
+  <si>
+    <t>variance is very high
+micro(93-56) and macro (77-16)</t>
+  </si>
+  <si>
+    <t>variance is very high
+micro(96-70) and macro (87-24)</t>
+  </si>
+  <si>
+    <t>output-61</t>
+  </si>
+  <si>
+    <t>output-62</t>
+  </si>
+  <si>
+    <t>output-63</t>
+  </si>
+  <si>
+    <t>output-64</t>
+  </si>
+  <si>
+    <t>output-65</t>
+  </si>
+  <si>
+    <t>output-66</t>
+  </si>
+  <si>
+    <t>10
+inh radius: 8</t>
+  </si>
+  <si>
+    <t>variance is high
+micro(100-33.3) and macro(33.3-0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30
+inh radius: 8 </t>
+  </si>
+  <si>
+    <t>variance is very high
+micro(97-61) and macro (57-0)</t>
+  </si>
+  <si>
+    <t>valid output but variance of micro is high
+micro(97-70) and macro(59-4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50
+inh radius: 8 </t>
+  </si>
+  <si>
+    <t>80
+inh radius: 8</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 120</t>
+  </si>
+  <si>
+    <t>valid output but variance of micro is high
+micro(89-65) and macro(56-13)</t>
+  </si>
+  <si>
+    <t>valid output
+micro(90-70) and macro(59-24)</t>
+  </si>
+  <si>
+    <t>100
+inh radius: 8</t>
+  </si>
+  <si>
+    <t>130
+inh radius: 8</t>
+  </si>
+  <si>
+    <t>32x32
+active col avg = 620</t>
+  </si>
+  <si>
+    <t>macro corelation is higher for cirlce-rectangle
+micro (94-76) and macro (80-56)</t>
   </si>
 </sst>
 </file>
@@ -349,7 +750,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -398,11 +799,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -411,6 +849,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -428,6 +878,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -709,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,33 +1180,42 @@
     <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="8" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="65.28515625" customWidth="1"/>
+    <col min="8" max="8" width="70.140625" customWidth="1"/>
     <col min="9" max="9" width="71.7109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="10" max="10" width="18.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="41.7109375" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="K1" s="17"/>
+      <c r="L1" s="18"/>
+    </row>
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
@@ -757,19 +1225,28 @@
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -782,23 +1259,23 @@
       <c r="D3" s="2">
         <v>0.1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="8">
         <v>-1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -811,23 +1288,23 @@
       <c r="D4" s="2">
         <v>0.3</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="8">
         <v>-1</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -840,23 +1317,23 @@
       <c r="D5" s="2">
         <v>0.5</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="8">
         <v>-1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -869,23 +1346,23 @@
       <c r="D6" s="2">
         <v>0.7</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="8">
         <v>-1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -898,23 +1375,23 @@
       <c r="D7" s="2">
         <v>0.9</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="8">
         <v>-1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -927,23 +1404,23 @@
       <c r="D8" s="2">
         <v>0.1</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="8">
         <v>-1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -956,23 +1433,23 @@
       <c r="D9" s="2">
         <v>0.3</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="8">
         <v>-1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -985,23 +1462,23 @@
       <c r="D10" s="2">
         <v>0.5</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="8">
         <v>-1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1014,23 +1491,23 @@
       <c r="D11" s="2">
         <v>0.7</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="8">
         <v>-1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1043,23 +1520,23 @@
       <c r="D12" s="2">
         <v>0.9</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="8">
         <v>-1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1072,23 +1549,23 @@
       <c r="D13" s="2">
         <v>0.1</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="8">
         <v>-1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1101,23 +1578,23 @@
       <c r="D14" s="2">
         <v>0.3</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="8">
         <v>-1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1130,23 +1607,23 @@
       <c r="D15" s="2">
         <v>0.5</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="8">
         <v>-1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1159,23 +1636,23 @@
       <c r="D16" s="2">
         <v>0.7</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="8">
         <v>-1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1188,23 +1665,23 @@
       <c r="D17" s="2">
         <v>0.9</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="8">
         <v>-1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -1217,23 +1694,33 @@
       <c r="D18" s="2">
         <v>0.1</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="8">
         <v>-1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="J18" s="2">
+        <v>89.65</v>
+      </c>
+      <c r="K18" s="2">
+        <v>80</v>
+      </c>
+      <c r="L18" s="2">
+        <v>67.56</v>
+      </c>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -1246,23 +1733,33 @@
       <c r="D19" s="2">
         <v>0.3</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="8">
         <v>-1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="J19" s="2">
+        <v>89.1</v>
+      </c>
+      <c r="K19" s="2">
+        <v>90.45</v>
+      </c>
+      <c r="L19" s="2">
+        <v>80</v>
+      </c>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -1275,23 +1772,33 @@
       <c r="D20" s="2">
         <v>0.5</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="8">
         <v>-1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="J20" s="2">
+        <v>94.64</v>
+      </c>
+      <c r="K20" s="2">
+        <v>96.7</v>
+      </c>
+      <c r="L20" s="2">
+        <v>94.52</v>
+      </c>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -1304,23 +1811,33 @@
       <c r="D21" s="2">
         <v>0.7</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="8">
         <v>-1</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="J21" s="2">
+        <v>94.76</v>
+      </c>
+      <c r="K21" s="2">
+        <v>97.98</v>
+      </c>
+      <c r="L21" s="2">
+        <v>96.018000000000001</v>
+      </c>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -1333,23 +1850,23 @@
       <c r="D22" s="2">
         <v>0.9</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="8">
         <v>-1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -1362,23 +1879,23 @@
       <c r="D23" s="2">
         <v>0.15</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="8">
         <v>-1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -1391,23 +1908,23 @@
       <c r="D24" s="2">
         <v>0.7</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="8">
         <v>-1</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -1420,23 +1937,23 @@
       <c r="D25" s="2">
         <v>0.5</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="8">
         <v>-1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -1449,23 +1966,23 @@
       <c r="D26" s="2">
         <v>0.3</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="8">
         <v>-1</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -1478,23 +1995,23 @@
       <c r="D27" s="2">
         <v>-1</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="8">
         <v>10</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -1507,23 +2024,23 @@
       <c r="D28" s="2">
         <v>-1</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="8">
         <v>20</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="I28" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -1536,23 +2053,23 @@
       <c r="D29" s="2">
         <v>-1</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="8">
         <v>50</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="I29" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -1565,23 +2082,23 @@
       <c r="D30" s="2">
         <v>-1</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="8">
         <v>100</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -1594,23 +2111,23 @@
       <c r="D31" s="2">
         <v>-1</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="8">
         <v>10</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -1623,23 +2140,23 @@
       <c r="D32" s="2">
         <v>-1</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="8">
         <v>50</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -1652,23 +2169,23 @@
       <c r="D33" s="2">
         <v>-1</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="8">
         <v>100</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -1681,23 +2198,23 @@
       <c r="D34" s="2">
         <v>-1</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="8">
         <v>100</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -1710,23 +2227,23 @@
       <c r="D35" s="2">
         <v>0.1</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="8">
         <v>-1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -1739,23 +2256,23 @@
       <c r="D36" s="2">
         <v>0.2</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="8">
         <v>-1</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -1768,28 +2285,1207 @@
       <c r="D37" s="2">
         <v>0.15</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="8">
         <v>-1</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I37" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2">
+        <v>5</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E38" s="8">
+        <v>-1</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J38" s="2">
+        <v>72.069999999999993</v>
+      </c>
+      <c r="K38" s="2">
+        <v>82.05</v>
+      </c>
+      <c r="L38" s="2">
+        <v>70.900000000000006</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" s="2">
+        <v>5</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E39" s="8">
+        <v>-1</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J39" s="2">
+        <v>82.46</v>
+      </c>
+      <c r="K39" s="2">
+        <v>86.22</v>
+      </c>
+      <c r="L39" s="2">
+        <v>77.83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40" s="2">
+        <v>5</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E40" s="8">
+        <v>-1</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J40" s="2">
+        <v>94.06</v>
+      </c>
+      <c r="K40" s="2">
+        <v>97.14</v>
+      </c>
+      <c r="L40" s="2">
+        <v>95.34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C41" s="2">
+        <v>5</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E41" s="8">
+        <v>-1</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J41" s="2">
+        <v>97.25</v>
+      </c>
+      <c r="K41" s="2">
+        <v>98.6</v>
+      </c>
+      <c r="L41" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2">
+        <v>5</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E42" s="8">
+        <v>-1</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J42" s="2">
+        <v>99.49</v>
+      </c>
+      <c r="K42" s="2">
+        <v>100</v>
+      </c>
+      <c r="L42" s="2">
+        <v>99.79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2">
+        <v>5</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E43" s="8">
+        <v>-1</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J43" s="2">
+        <v>95.09</v>
+      </c>
+      <c r="K43" s="2">
+        <v>94.11</v>
+      </c>
+      <c r="L43" s="2">
+        <v>87.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2">
+        <v>5</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E44" s="8">
+        <v>-1</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J44" s="2">
+        <v>97.39</v>
+      </c>
+      <c r="K44" s="2">
+        <v>97.71</v>
+      </c>
+      <c r="L44" s="2">
+        <v>92.18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2">
+        <v>5</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E45" s="8">
+        <v>-1</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J45" s="2">
+        <v>93.35</v>
+      </c>
+      <c r="K45" s="2">
+        <v>98.24</v>
+      </c>
+      <c r="L45" s="2">
+        <v>91.01</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2">
+        <v>5</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E46" s="8">
+        <v>-1</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J46" s="2">
+        <v>96.78</v>
+      </c>
+      <c r="K46" s="2">
+        <v>98.74</v>
+      </c>
+      <c r="L46" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2">
+        <v>5</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E47" s="8">
+        <v>-1</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J47" s="2">
+        <v>100</v>
+      </c>
+      <c r="K47" s="2">
+        <v>99.67</v>
+      </c>
+      <c r="L47" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C48" s="2">
+        <v>5</v>
+      </c>
+      <c r="D48" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J48" s="2">
+        <v>76.64</v>
+      </c>
+      <c r="K48" s="2">
+        <v>81.63</v>
+      </c>
+      <c r="L48" s="2">
+        <v>78.010000000000005</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C49" s="2">
+        <v>5</v>
+      </c>
+      <c r="D49" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J49" s="2">
+        <v>84.83</v>
+      </c>
+      <c r="K49" s="2">
+        <v>91.51</v>
+      </c>
+      <c r="L49" s="2">
+        <v>81.67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C50" s="2">
+        <v>5</v>
+      </c>
+      <c r="D50" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J50" s="2">
+        <v>93.9</v>
+      </c>
+      <c r="K50" s="2">
+        <v>96.2</v>
+      </c>
+      <c r="L50" s="2">
+        <v>95.48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>49</v>
+      </c>
+      <c r="B51" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C51" s="2">
+        <v>5</v>
+      </c>
+      <c r="D51" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J51" s="2">
+        <v>93.79</v>
+      </c>
+      <c r="K51" s="2">
+        <v>96.5</v>
+      </c>
+      <c r="L51" s="2">
+        <v>95.72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C52" s="2">
+        <v>5</v>
+      </c>
+      <c r="D52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J52" s="2">
+        <v>93.79</v>
+      </c>
+      <c r="K52" s="2">
+        <v>96.76</v>
+      </c>
+      <c r="L52" s="2">
+        <v>95.73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>51</v>
+      </c>
+      <c r="B53" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C53" s="2">
+        <v>5</v>
+      </c>
+      <c r="D53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J53" s="2">
+        <v>85.76</v>
+      </c>
+      <c r="K53" s="2">
+        <v>85.61</v>
+      </c>
+      <c r="L53" s="2">
+        <v>78.040000000000006</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>52</v>
+      </c>
+      <c r="B54" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C54" s="2">
+        <v>5</v>
+      </c>
+      <c r="D54" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J54" s="2">
+        <v>93.38</v>
+      </c>
+      <c r="K54" s="2">
+        <v>94.04</v>
+      </c>
+      <c r="L54" s="2">
+        <v>93.46</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>53</v>
+      </c>
+      <c r="B55" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C55" s="2">
+        <v>5</v>
+      </c>
+      <c r="D55" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J55" s="2">
+        <v>87.21</v>
+      </c>
+      <c r="K55" s="2">
+        <v>92.9</v>
+      </c>
+      <c r="L55" s="2">
+        <v>85.9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>54</v>
+      </c>
+      <c r="B56" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C56" s="2">
+        <v>5</v>
+      </c>
+      <c r="D56" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J56" s="2">
+        <v>80</v>
+      </c>
+      <c r="K56" s="2">
+        <v>40</v>
+      </c>
+      <c r="L56" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2">
+        <v>5</v>
+      </c>
+      <c r="D57" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J57" s="2">
+        <v>85</v>
+      </c>
+      <c r="K57" s="2">
+        <v>70</v>
+      </c>
+      <c r="L57" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>56</v>
+      </c>
+      <c r="B58" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C58" s="2">
+        <v>5</v>
+      </c>
+      <c r="D58" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J58" s="2">
+        <v>83.33</v>
+      </c>
+      <c r="K58" s="2">
+        <v>80</v>
+      </c>
+      <c r="L58" s="2">
+        <v>53.33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C59" s="2">
+        <v>5</v>
+      </c>
+      <c r="D59" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="J59" s="2">
+        <v>85</v>
+      </c>
+      <c r="K59" s="2">
+        <v>85</v>
+      </c>
+      <c r="L59" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>58</v>
+      </c>
+      <c r="B60" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C60" s="2">
+        <v>5</v>
+      </c>
+      <c r="D60" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J60" s="2">
+        <v>84</v>
+      </c>
+      <c r="K60" s="2">
+        <v>88</v>
+      </c>
+      <c r="L60" s="2">
         <v>74</v>
       </c>
     </row>
+    <row r="61" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>59</v>
+      </c>
+      <c r="B61" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C61" s="2">
+        <v>5</v>
+      </c>
+      <c r="D61" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J61" s="2">
+        <v>91.25</v>
+      </c>
+      <c r="K61" s="2">
+        <v>92.5</v>
+      </c>
+      <c r="L61" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>60</v>
+      </c>
+      <c r="B62" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C62" s="2">
+        <v>5</v>
+      </c>
+      <c r="D62" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J62" s="2">
+        <v>95</v>
+      </c>
+      <c r="K62" s="2">
+        <v>96</v>
+      </c>
+      <c r="L62" s="2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>61</v>
+      </c>
+      <c r="B63" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C63" s="2">
+        <v>10</v>
+      </c>
+      <c r="D63" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J63" s="2">
+        <v>90</v>
+      </c>
+      <c r="K63" s="2">
+        <v>71.8</v>
+      </c>
+      <c r="L63" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>62</v>
+      </c>
+      <c r="B64" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C64" s="2">
+        <v>10</v>
+      </c>
+      <c r="D64" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J64" s="2">
+        <v>93.33</v>
+      </c>
+      <c r="K64" s="2">
+        <v>80.55</v>
+      </c>
+      <c r="L64" s="2">
+        <v>65.78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>63</v>
+      </c>
+      <c r="B65" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C65" s="2">
+        <v>10</v>
+      </c>
+      <c r="D65" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="J65" s="2">
+        <v>92</v>
+      </c>
+      <c r="K65" s="2">
+        <v>85.5</v>
+      </c>
+      <c r="L65" s="2">
+        <v>76.38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>64</v>
+      </c>
+      <c r="B66" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C66" s="2">
+        <v>10</v>
+      </c>
+      <c r="D66" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J66" s="2">
+        <v>88.6</v>
+      </c>
+      <c r="K66" s="2">
+        <v>89.69</v>
+      </c>
+      <c r="L66" s="2">
+        <v>78.62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>65</v>
+      </c>
+      <c r="B67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C67" s="2">
+        <v>10</v>
+      </c>
+      <c r="D67" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="J67" s="2">
+        <v>82.03</v>
+      </c>
+      <c r="K67" s="2">
+        <v>89.25</v>
+      </c>
+      <c r="L67" s="2">
+        <v>81.599999999999994</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>65</v>
+      </c>
+      <c r="B68" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C68" s="2">
+        <v>10</v>
+      </c>
+      <c r="D68" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="J68" s="2">
+        <v>94.5</v>
+      </c>
+      <c r="K68" s="2">
+        <v>93.5</v>
+      </c>
+      <c r="L68" s="2">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="J1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>